<commit_message>
Estudando Python com Excel em 10/06
</commit_message>
<xml_diff>
--- a/Mod_8_Excel_Avancado/Quebrar.xlsx
+++ b/Mod_8_Excel_Avancado/Quebrar.xlsx
@@ -3,14 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Amanda Martins" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Eliane Moreira" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Leonardo Almeida" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nicolas Pereira" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -434,7 +430,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -690,208 +686,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Produtos</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Vendas</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Amanda Martins</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Bolsa de Trabalho</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>248.73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Produtos</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Vendas</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Eliane Moreira</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Calça Feminina Jogger</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>69.98999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Produtos</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Vendas</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Leonardo Almeida</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Tênis Feminino</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>89.98999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Produtos</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Vendas</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Nicolas Pereira</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Camisa Masculina</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>153.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>